<commit_message>
big changes incoming. see Changes to EBT march 2025.docx
</commit_message>
<xml_diff>
--- a/config/reference_table_fuel.xlsx
+++ b/config/reference_table_fuel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finbar.maunsell\github\Outlook9th_EBT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137230B0-F2D1-43A6-B7C7-26584CF55179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CEAA00-C985-44C4-A27F-141435BE1D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="1485" windowWidth="19425" windowHeight="10305" xr2:uid="{5F1DA014-A728-4F9E-B214-74A475618C33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5F1DA014-A728-4F9E-B214-74A475618C33}"/>
   </bookViews>
   <sheets>
     <sheet name="fuels" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="94">
   <si>
     <t>unique_the_end_of_fuels</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>13_tide_wave_ocean</t>
-  </si>
-  <si>
-    <t>(minus)</t>
   </si>
   <si>
     <t>14_wind</t>
@@ -359,7 +356,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,12 +378,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,7 +429,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -446,17 +437,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -867,32 +857,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810C7032-4F78-4575-8697-E23599D6D314}">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="37.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="37.125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="37.125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="37.125" style="9" customWidth="1"/>
     <col min="5" max="5" width="34.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -904,7 +894,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
@@ -915,7 +905,7 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
@@ -923,13 +913,13 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -939,7 +929,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
@@ -948,7 +938,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
@@ -959,7 +949,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
@@ -970,7 +960,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
@@ -981,8 +971,8 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="7" t="s">
-        <v>74</v>
+      <c r="E9" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -994,8 +984,8 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="7" t="s">
-        <v>74</v>
+      <c r="E10" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1007,7 +997,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
@@ -1018,7 +1008,7 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
@@ -1029,7 +1019,7 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
@@ -1040,38 +1030,38 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="8" t="s">
-        <v>76</v>
+      <c r="C15" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
@@ -1082,7 +1072,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
@@ -1093,7 +1083,7 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
@@ -1104,7 +1094,7 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
@@ -1115,29 +1105,29 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="9" t="s">
-        <v>77</v>
+      <c r="C22" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="7"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
@@ -1148,7 +1138,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
@@ -1159,7 +1149,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="7"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
@@ -1170,7 +1160,7 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="7"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
@@ -1181,18 +1171,18 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="7"/>
+      <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="7"/>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
@@ -1203,7 +1193,7 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="7"/>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
@@ -1211,10 +1201,10 @@
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="7"/>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
@@ -1223,7 +1213,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="7"/>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
@@ -1232,7 +1222,7 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="7"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="4" t="s">
@@ -1241,7 +1231,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="7"/>
+      <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
@@ -1250,7 +1240,7 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="7"/>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="4" t="s">
@@ -1259,7 +1249,7 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="7"/>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
@@ -1270,7 +1260,7 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="7"/>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
@@ -1281,7 +1271,7 @@
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="7"/>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
@@ -1292,7 +1282,7 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="7"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
@@ -1303,7 +1293,7 @@
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="7"/>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
@@ -1314,7 +1304,7 @@
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="7"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
@@ -1325,7 +1315,7 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="7"/>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
@@ -1336,42 +1326,40 @@
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="7"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="7"/>
+      <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="7"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="1"/>
-      <c r="B45" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E45" s="7"/>
+      <c r="A45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
@@ -1382,412 +1370,412 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="7"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="7"/>
+      <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="7"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="7"/>
+      <c r="E49" s="6"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="7"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="7"/>
+      <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="7"/>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="7"/>
+      <c r="E53" s="6"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="7"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="7"/>
+      <c r="E55" s="6"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="7"/>
+      <c r="E56" s="6"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="7"/>
+      <c r="E57" s="6"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="7"/>
+      <c r="E58" s="6"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="7"/>
+      <c r="E59" s="6"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="7"/>
+      <c r="E60" s="6"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="7"/>
+      <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="7"/>
+      <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="7"/>
+      <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="7"/>
+      <c r="E64" s="6"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>86</v>
+        <v>66</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="7"/>
+      <c r="E66" s="6"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
-      <c r="E67" s="7"/>
+      <c r="E67" s="6"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
-      <c r="E68" s="7"/>
+      <c r="E68" s="6"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="7"/>
+      <c r="E69" s="6"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B71" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C71" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E70" s="7"/>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="D71" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E71" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="E71" s="6"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B73" s="12" t="s">
+      <c r="B74" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C73" s="12" t="s">
+      <c r="C74" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E73" s="7"/>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="12" t="s">
+      <c r="D74" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B74" s="12" t="s">
+      <c r="B75" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C74" s="12" t="s">
+      <c r="C75" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E74" s="7"/>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="12" t="s">
+      <c r="D75" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B75" s="12" t="s">
+      <c r="B76" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C76" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="12" t="s">
+      <c r="D76" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B76" s="12" t="s">
+      <c r="B77" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C77" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="12" t="s">
+      <c r="D77" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B77" s="12" t="s">
+      <c r="B78" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C78" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="12" t="s">
+      <c r="D78" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B79" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C79" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B79" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C79" s="12" t="s">
-        <v>94</v>
-      </c>
       <c r="D79" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1811,6 +1799,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3042e625-934f-4bb2-8533-cbb6446c8b2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010033DE4B8CEBD9304286F1E0B7BC383844" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d76399d66d45378b52bd24e5db7672eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa" xmlns:ns3="3042e625-934f-4bb2-8533-cbb6446c8b2b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f81e3bb06f6900da50fdd409f0138bcf" ns2:_="" ns3:_="">
     <xsd:import namespace="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
@@ -2021,17 +2020,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3042e625-934f-4bb2-8533-cbb6446c8b2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2042,6 +2030,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5237F13-F310-44F8-BFDB-5B30CCBA5B0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
+    <ds:schemaRef ds:uri="3042e625-934f-4bb2-8533-cbb6446c8b2b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9642CE3B-4FD3-4124-99D4-C3CA26C580C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2060,17 +2059,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5237F13-F310-44F8-BFDB-5B30CCBA5B0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="339e5aef-327d-4eb6-a8e0-9b2fd01ac0fa"/>
-    <ds:schemaRef ds:uri="3042e625-934f-4bb2-8533-cbb6446c8b2b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33D62E73-70C8-4A61-97EF-BB6671B92616}">
   <ds:schemaRefs>

</xml_diff>